<commit_message>
Wrote in wrong Excel document. Updated data in correct one.
</commit_message>
<xml_diff>
--- a/Exercise3/Multiplication/Mappe1.xlsx
+++ b/Exercise3/Multiplication/Mappe1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Universitet\Elektronik\2. semester\DSD\Exercise3\Multiplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Universitet\Elektronik\2. semester\DSD\Exercise2-4\Exercise3\Multiplication\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Input bit size</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t># of LE's</t>
+  </si>
+  <si>
+    <t>Constant</t>
   </si>
 </sst>
 </file>
@@ -208,11 +211,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1316957136"/>
-        <c:axId val="1316961488"/>
+        <c:axId val="1100550768"/>
+        <c:axId val="1100548048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1316957136"/>
+        <c:axId val="1100550768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -330,12 +333,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1316961488"/>
+        <c:crossAx val="1100548048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1316961488"/>
+        <c:axId val="1100548048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,7 +451,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1316957136"/>
+        <c:crossAx val="1100550768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1057,16 +1060,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1351,15 +1354,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1369,8 +1372,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1380,8 +1389,14 @@
       <c r="C2">
         <v>103</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -1391,8 +1406,14 @@
       <c r="C3">
         <v>75</v>
       </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1402,8 +1423,14 @@
       <c r="C4">
         <v>63</v>
       </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1413,8 +1440,14 @@
       <c r="C5">
         <v>41</v>
       </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1424,8 +1457,14 @@
       <c r="C6">
         <v>31</v>
       </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1435,8 +1474,14 @@
       <c r="C7">
         <v>17</v>
       </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1446,8 +1491,14 @@
       <c r="C8">
         <v>4</v>
       </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1456,6 +1507,68 @@
       </c>
       <c r="C9">
         <v>1</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before start of exercise 4
</commit_message>
<xml_diff>
--- a/Exercise3/Multiplication/Mappe1.xlsx
+++ b/Exercise3/Multiplication/Mappe1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Input bit size</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>Constant</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Expected # of LE's</t>
   </si>
 </sst>
 </file>
@@ -113,6 +119,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v># of LE's</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -137,66 +146,198 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$A$2:$A$9</c:f>
+              <c:f>'Ark1'!$M$2:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$C$2:$C$9</c:f>
+              <c:f>'Ark1'!$O$2:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>103</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>583</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Expected</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ark1'!$M$2:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>75</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ark1'!$P$2:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -211,13 +352,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1100550768"/>
-        <c:axId val="1100548048"/>
+        <c:axId val="-1427313168"/>
+        <c:axId val="-1427305552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1100550768"/>
+        <c:axId val="-1427313168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -333,14 +475,15 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100548048"/>
+        <c:crossAx val="-1427305552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1100548048"/>
+        <c:axId val="-1427305552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="600"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -451,7 +594,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100550768"/>
+        <c:crossAx val="-1427313168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -463,6 +606,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1061,15 +1236,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90854</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>167054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1354,208 +1529,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="J1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="E1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
       </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>103</v>
-      </c>
+    <row r="2" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <f>M2^2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <f>O2-P2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>75</v>
-      </c>
+    <row r="3" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J3">
         <v>2</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P13" si="0">M3^2</f>
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q13" si="1">O3-P3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>63</v>
-      </c>
+    <row r="4" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4">
         <v>9</v>
       </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <v>17</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>41</v>
-      </c>
+    <row r="5" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J5">
         <v>4</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
+        <v>31</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>31</v>
-      </c>
+    <row r="6" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6">
         <v>9</v>
       </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>41</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>17</v>
-      </c>
+    <row r="7" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J7">
         <v>6</v>
       </c>
       <c r="K7">
         <v>9</v>
       </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>12</v>
+      </c>
+      <c r="O7">
+        <v>63</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
+    <row r="8" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J8">
         <v>7</v>
       </c>
       <c r="K8">
         <v>17</v>
       </c>
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>14</v>
+      </c>
+      <c r="O8">
+        <v>75</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
+    <row r="9" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J9">
         <v>8</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9">
+        <v>16</v>
+      </c>
+      <c r="O9">
+        <v>103</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>9</v>
       </c>
       <c r="K10">
         <v>9</v>
       </c>
+      <c r="M10">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>18</v>
+      </c>
+      <c r="O10">
+        <v>116</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>10</v>
       </c>
       <c r="K11">
         <v>9</v>
       </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>20</v>
+      </c>
+      <c r="O11">
+        <v>151</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>11</v>
       </c>
       <c r="K12">
         <v>22</v>
       </c>
+      <c r="M12">
+        <v>20</v>
+      </c>
+      <c r="N12">
+        <v>40</v>
+      </c>
+      <c r="O12">
+        <v>583</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J13">
         <v>12</v>
       </c>
       <c r="K13">
         <v>9</v>
       </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <v>200</v>
+      </c>
+      <c r="O13">
+        <v>13867</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>3867</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J14">
         <v>13</v>
       </c>
       <c r="K14">
         <v>20</v>
       </c>
+      <c r="M14">
+        <v>1000</v>
+      </c>
+      <c r="N14">
+        <f>M14^2</f>
+        <v>1000000</v>
+      </c>
+      <c r="O14">
+        <v>342999</v>
+      </c>
+      <c r="P14">
+        <f>M14^2</f>
+        <v>1000000</v>
+      </c>
+      <c r="Q14">
+        <f>O14-P14</f>
+        <v>-657001</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J15">
         <v>14</v>
       </c>
@@ -1563,7 +1894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J16">
         <v>15</v>
       </c>

</xml_diff>